<commit_message>
fix file checklist, add date and name
</commit_message>
<xml_diff>
--- a/security/checklist_security-lab3.xlsx
+++ b/security/checklist_security-lab3.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Tên project</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Câu 3:
 - Màn hình update
 - Thiết lập giá trị name là: giá trị trong ngoặc  (      ) (chỉ copy giá trị trong ngoặc , không bao gồm dấu ngoặc
@@ -160,6 +166,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Câu 3:
 - Màn hình update
 - Thiết lập giá trị name là: giá trị trong ngoặc  (</t>
@@ -197,6 +209,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Câu 3:
 - Màn hình update
 - Thiết lập giá trị name là: giá trị trong ngoặc  (</t>
@@ -234,6 +252,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Câu 3:
 - Màn hình update
 - Thiết lập giá trị name là: giá trị trong ngoặc  (</t>
@@ -343,6 +367,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t>Câu 3:
 - Màn hình update
 - Thiết lập giá trị name là: giá trị trong ngoặc  (ABCDE) (chỉ copy giá trị trong ngoặc , không bao gồm dấu ngoặc
@@ -699,16 +729,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1875,9 +1905,9 @@
   <dimension ref="A1:AE898"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AG10" sqref="AG10"/>
+      <selection pane="bottomLeft" activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4351851851852" defaultRowHeight="15.75" customHeight="1"/>
@@ -2098,8 +2128,12 @@
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
       <c r="W6" s="13"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="25"/>
+      <c r="X6" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y6" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z6" s="25" t="s">
         <v>25</v>
       </c>
@@ -2140,8 +2174,12 @@
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
       <c r="W7" s="13"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="25"/>
+      <c r="X7" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y7" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z7" s="25" t="s">
         <v>25</v>
       </c>
@@ -2182,8 +2220,12 @@
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
       <c r="W8" s="13"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="25"/>
+      <c r="X8" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y8" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z8" s="25" t="s">
         <v>25</v>
       </c>
@@ -2223,8 +2265,12 @@
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="25"/>
+      <c r="X9" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y9" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z9" s="25" t="s">
         <v>25</v>
       </c>
@@ -2265,8 +2311,12 @@
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
       <c r="W10" s="13"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="25"/>
+      <c r="X10" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y10" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z10" s="25" t="s">
         <v>25</v>
       </c>
@@ -2307,8 +2357,12 @@
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="25"/>
+      <c r="X11" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y11" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z11" s="25" t="s">
         <v>25</v>
       </c>
@@ -2349,8 +2403,12 @@
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
       <c r="W12" s="13"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="25"/>
+      <c r="X12" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y12" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z12" s="25" t="s">
         <v>25</v>
       </c>
@@ -2391,8 +2449,12 @@
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
       <c r="W13" s="13"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="25"/>
+      <c r="X13" s="18">
+        <v>45568</v>
+      </c>
+      <c r="Y13" s="25" t="s">
+        <v>24</v>
+      </c>
       <c r="Z13" s="25" t="s">
         <v>25</v>
       </c>

</xml_diff>